<commit_message>
changing PD to MARKAL 2050 value (FY21-EMANES3) of 104512 MW
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_Master_LC_GEP_original.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_Master_LC_GEP_original.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660F1261-3806-409B-BA30-8BD942E72BD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED57D2C4-988B-4931-A952-AA2E79E1CCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="927" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="927" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LC_GEP Setting" sheetId="1" r:id="rId1"/>
@@ -18,39 +18,66 @@
     <sheet name="Simulation Setting" sheetId="3" r:id="rId3"/>
     <sheet name="Simulation Configuration" sheetId="4" r:id="rId4"/>
     <sheet name="Gen Technology" sheetId="5" r:id="rId5"/>
-    <sheet name="File Path" sheetId="6" r:id="rId6"/>
-    <sheet name="Scenario Reduction Setting" sheetId="7" r:id="rId7"/>
-    <sheet name="ATB Setting" sheetId="8" r:id="rId8"/>
-    <sheet name="Ancillary Tabs-&gt;" sheetId="9" r:id="rId9"/>
-    <sheet name="ATB List" sheetId="10" r:id="rId10"/>
+    <sheet name="Gen Technology (2)" sheetId="11" r:id="rId6"/>
+    <sheet name="File Path" sheetId="6" r:id="rId7"/>
+    <sheet name="Scenario Reduction Setting" sheetId="7" r:id="rId8"/>
+    <sheet name="ATB Setting" sheetId="8" r:id="rId9"/>
+    <sheet name="Ancillary Tabs-&gt;" sheetId="9" r:id="rId10"/>
+    <sheet name="ATB List" sheetId="10" r:id="rId11"/>
   </sheets>
   <definedNames>
+    <definedName name="Battery" localSheetId="5">Table2[Battery]</definedName>
     <definedName name="Battery">Table2[Battery]</definedName>
+    <definedName name="Battery_Tech" localSheetId="5">Table2[Battery]</definedName>
     <definedName name="Battery_Tech">Table2[Battery]</definedName>
+    <definedName name="Biopower" localSheetId="5">Table3[Biopower]</definedName>
     <definedName name="Biopower">Table3[Biopower]</definedName>
+    <definedName name="Biopower_Tech" localSheetId="5">Table3[Biopower]</definedName>
     <definedName name="Biopower_Tech">Table3[Biopower]</definedName>
+    <definedName name="Coal" localSheetId="5">Table4[Coal]</definedName>
     <definedName name="Coal">Table4[Coal]</definedName>
+    <definedName name="Coal_Tech" localSheetId="5">Table4[Coal]</definedName>
     <definedName name="Coal_Tech">Table4[Coal]</definedName>
+    <definedName name="CommPV" localSheetId="5">Table5[CommPV]</definedName>
     <definedName name="CommPV">Table5[CommPV]</definedName>
+    <definedName name="CommPV_Tech" localSheetId="5">Table5[CommPV]</definedName>
     <definedName name="CommPV_Tech">Table5[CommPV]</definedName>
+    <definedName name="CSP" localSheetId="5">Table6[CSP]</definedName>
     <definedName name="CSP">Table6[CSP]</definedName>
+    <definedName name="CSP_Tech" localSheetId="5">Table6[CSP]</definedName>
     <definedName name="CSP_Tech">Table6[CSP]</definedName>
+    <definedName name="Geothermal" localSheetId="5">Table7[Geothermal]</definedName>
     <definedName name="Geothermal">Table7[Geothermal]</definedName>
+    <definedName name="Geothermal_Tech" localSheetId="5">Table7[Geothermal]</definedName>
     <definedName name="Geothermal_Tech">Table7[Geothermal]</definedName>
+    <definedName name="Hydropower" localSheetId="5">Table8[Hydropower]</definedName>
     <definedName name="Hydropower">Table8[Hydropower]</definedName>
+    <definedName name="Hydropower_Tech" localSheetId="5">Table8[Hydropower]</definedName>
     <definedName name="Hydropower_Tech">Table8[Hydropower]</definedName>
+    <definedName name="LandbasedWind" localSheetId="5">Table9[LandbasedWind]</definedName>
     <definedName name="LandbasedWind">Table9[LandbasedWind]</definedName>
+    <definedName name="LandWind_Tech" localSheetId="5">Table9[LandbasedWind]</definedName>
     <definedName name="LandWind_Tech">Table9[LandbasedWind]</definedName>
+    <definedName name="NaturalGas" localSheetId="5">Table10[NaturalGas]</definedName>
     <definedName name="NaturalGas">Table10[NaturalGas]</definedName>
+    <definedName name="Nuclear" localSheetId="5">Table11[Nuclear]</definedName>
     <definedName name="Nuclear">Table11[Nuclear]</definedName>
+    <definedName name="Nuclear_Tech" localSheetId="5">Table11[Nuclear]</definedName>
     <definedName name="Nuclear_Tech">Table11[Nuclear]</definedName>
+    <definedName name="OffShoreWind" localSheetId="5">Table12[OffShoreWind]</definedName>
     <definedName name="OffShoreWind">Table12[OffShoreWind]</definedName>
+    <definedName name="OffShoreWind_Tech" localSheetId="5">Table12[OffShoreWind]</definedName>
     <definedName name="OffShoreWind_Tech">Table12[OffShoreWind]</definedName>
+    <definedName name="ResPV" localSheetId="5">Table13[ResPV]</definedName>
     <definedName name="ResPV">Table13[ResPV]</definedName>
     <definedName name="ResPV_Tech">'ATB List'!$T$2:$T$6</definedName>
+    <definedName name="Tech_Data" localSheetId="5">Table16[]</definedName>
     <definedName name="Tech_Data">Table16[]</definedName>
+    <definedName name="Technology" localSheetId="5">Table1[Tech]</definedName>
     <definedName name="Technology">Table1[Tech]</definedName>
+    <definedName name="UtilityPV" localSheetId="5">Table14[UtilityPV]</definedName>
     <definedName name="UtilityPV">Table14[UtilityPV]</definedName>
+    <definedName name="UtilityPV_Tech" localSheetId="5">Table14[UtilityPV]</definedName>
     <definedName name="UtilityPV_Tech">Table14[UtilityPV]</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -69,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="316">
   <si>
     <t>Setting</t>
   </si>
@@ -1091,6 +1118,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1382,7 +1410,107 @@
     <cellStyle name="Normal 5" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Output" xfId="10" builtinId="21"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" indent="1"/>
     </dxf>
@@ -1644,66 +1772,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1718,22 +1786,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table15" displayName="Table15" ref="A1:M15" totalsRowShown="0" dataDxfId="15" headerRowBorderDxfId="16" headerRowCellStyle="Heading 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table15" displayName="Table15" ref="A1:M15" totalsRowShown="0" dataDxfId="25" headerRowBorderDxfId="26" headerRowCellStyle="Heading 3">
   <autoFilter ref="A1:M15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ATB_Setting_ID" dataDxfId="14" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tech_ID" dataDxfId="13" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="UNITGROUP" dataDxfId="12" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="UNIT_CATEGORY" dataDxfId="11" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="UNIT_TYPE" dataDxfId="10" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="FUEL" dataDxfId="9" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tech" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="TechDetail" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Case" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="CRP" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Scenario" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Year" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="ATB Year" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ATB_Setting_ID" dataDxfId="24" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tech_ID" dataDxfId="23" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="UNITGROUP" dataDxfId="22" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="UNIT_CATEGORY" dataDxfId="21" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="UNIT_TYPE" dataDxfId="20" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="FUEL" dataDxfId="19" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tech" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="TechDetail" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Case" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="CRP" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Scenario" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Year" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="ATB Year" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1822,10 +1890,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table2" displayName="Table2" ref="I1:I6" totalsRowShown="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table2" displayName="Table2" ref="I1:I6" totalsRowShown="0" dataDxfId="11">
   <autoFilter ref="I1:I6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Battery" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Battery" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2227,6 +2295,23 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S37" sqref="S37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Z213"/>
   <sheetViews>
@@ -5442,8 +5527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5944,7 +6029,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E3">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5957,10 +6042,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AL8"/>
+  <dimension ref="A1:AL6"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AG7" sqref="AG7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6091,6 +6176,775 @@
     </row>
     <row r="2" spans="1:38">
       <c r="A2" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="23">
+        <v>100</v>
+      </c>
+      <c r="G2" s="23">
+        <v>0</v>
+      </c>
+      <c r="H2" s="23">
+        <v>1</v>
+      </c>
+      <c r="I2" s="26">
+        <v>0</v>
+      </c>
+      <c r="J2" s="23">
+        <v>0</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="L2" s="23">
+        <v>0</v>
+      </c>
+      <c r="M2" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="N2" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="P2" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="23">
+        <v>0</v>
+      </c>
+      <c r="R2" s="23">
+        <v>0</v>
+      </c>
+      <c r="S2" s="24">
+        <v>3.4119999999999999</v>
+      </c>
+      <c r="T2" s="23">
+        <v>1</v>
+      </c>
+      <c r="U2" s="23">
+        <v>1</v>
+      </c>
+      <c r="V2" s="26">
+        <v>0</v>
+      </c>
+      <c r="W2" s="26">
+        <v>0</v>
+      </c>
+      <c r="X2" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="26">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="Z2" s="23">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="23">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="AD2" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="23">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="23">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="AL2" s="24"/>
+    </row>
+    <row r="3" spans="1:38">
+      <c r="A3" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="F3" s="23">
+        <v>100</v>
+      </c>
+      <c r="G3" s="23">
+        <v>0</v>
+      </c>
+      <c r="H3" s="23">
+        <v>1</v>
+      </c>
+      <c r="I3" s="26">
+        <v>0</v>
+      </c>
+      <c r="J3" s="23">
+        <v>0</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="L3" s="23">
+        <v>0</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="N3" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="P3" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="23">
+        <v>0</v>
+      </c>
+      <c r="R3" s="23">
+        <v>0</v>
+      </c>
+      <c r="S3" s="24">
+        <v>3.4119999999999999</v>
+      </c>
+      <c r="T3" s="23">
+        <v>1</v>
+      </c>
+      <c r="U3" s="23">
+        <v>1</v>
+      </c>
+      <c r="V3" s="26">
+        <v>0</v>
+      </c>
+      <c r="W3" s="26">
+        <v>0</v>
+      </c>
+      <c r="X3" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="26">
+        <v>0.75</v>
+      </c>
+      <c r="Z3" s="23">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="23">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="AD3" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="23">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="23">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="AL3" s="24"/>
+    </row>
+    <row r="4" spans="1:38">
+      <c r="A4" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="F4" s="23">
+        <v>1000</v>
+      </c>
+      <c r="G4" s="23">
+        <v>0</v>
+      </c>
+      <c r="H4" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="I4" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="J4" s="23">
+        <v>0</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="L4" s="23">
+        <v>0</v>
+      </c>
+      <c r="M4" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="O4" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="P4" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="23">
+        <v>0</v>
+      </c>
+      <c r="R4" s="23">
+        <v>0</v>
+      </c>
+      <c r="S4" s="24">
+        <v>10.461</v>
+      </c>
+      <c r="T4" s="23">
+        <v>0</v>
+      </c>
+      <c r="U4" s="23">
+        <v>0</v>
+      </c>
+      <c r="V4" s="26">
+        <v>0</v>
+      </c>
+      <c r="W4" s="26">
+        <v>0</v>
+      </c>
+      <c r="X4" s="26">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="Z4" s="23">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="23">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="AD4" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="23">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="23">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="AL4" s="24"/>
+    </row>
+    <row r="5" spans="1:38">
+      <c r="A5" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" s="23">
+        <v>200</v>
+      </c>
+      <c r="G5" s="23">
+        <v>0</v>
+      </c>
+      <c r="H5" s="23">
+        <v>0.9</v>
+      </c>
+      <c r="I5" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="J5" s="23">
+        <v>0</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="L5" s="23">
+        <v>0</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="O5" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="P5" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="23">
+        <v>0</v>
+      </c>
+      <c r="R5" s="23">
+        <v>0</v>
+      </c>
+      <c r="S5" s="24">
+        <v>6.4009999999999998</v>
+      </c>
+      <c r="T5" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="U5" s="23">
+        <v>0.6</v>
+      </c>
+      <c r="V5" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="W5" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="X5" s="26">
+        <v>0.35</v>
+      </c>
+      <c r="Y5" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="Z5" s="23">
+        <v>53.18</v>
+      </c>
+      <c r="AA5" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="23">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="AD5" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="23">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="23">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="AL5" s="24"/>
+    </row>
+    <row r="6" spans="1:38">
+      <c r="A6" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" s="23">
+        <v>50</v>
+      </c>
+      <c r="G6" s="23">
+        <v>0</v>
+      </c>
+      <c r="H6" s="23">
+        <v>0.92</v>
+      </c>
+      <c r="I6" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="23">
+        <v>0</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="L6" s="23">
+        <v>0</v>
+      </c>
+      <c r="M6" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="N6" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="O6" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="P6" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="23">
+        <v>0</v>
+      </c>
+      <c r="R6" s="23">
+        <v>0</v>
+      </c>
+      <c r="S6" s="24">
+        <v>9.5150000000000006</v>
+      </c>
+      <c r="T6" s="23">
+        <v>1</v>
+      </c>
+      <c r="U6" s="23">
+        <v>1</v>
+      </c>
+      <c r="V6" s="26">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="W6" s="26">
+        <v>0.83</v>
+      </c>
+      <c r="X6" s="26">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="26">
+        <v>0.92</v>
+      </c>
+      <c r="Z6" s="23">
+        <v>53.18</v>
+      </c>
+      <c r="AA6" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="23">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="AD6" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="23">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="23">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AK6" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="AL6" s="24"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="AJ2">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ3">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ4:AJ6">
+    <cfRule type="cellIs" dxfId="1" priority="19" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD2:AG6">
+    <cfRule type="cellIs" dxfId="0" priority="23" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D07519-F835-4C19-99E7-06F78FDFB654}">
+  <dimension ref="A1:AL8"/>
+  <sheetViews>
+    <sheetView topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AD18" sqref="AD18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="3" width="16.59765625" customWidth="1"/>
+    <col min="4" max="4" width="13.1328125" customWidth="1"/>
+    <col min="6" max="7" width="12" customWidth="1"/>
+    <col min="22" max="22" width="17.1328125" customWidth="1"/>
+    <col min="23" max="24" width="11.59765625" customWidth="1"/>
+    <col min="25" max="25" width="13.59765625" customWidth="1"/>
+    <col min="26" max="28" width="11.59765625" customWidth="1"/>
+    <col min="29" max="29" width="13.265625" customWidth="1"/>
+    <col min="30" max="30" width="20.1328125" customWidth="1"/>
+    <col min="31" max="31" width="15.265625" customWidth="1"/>
+    <col min="32" max="32" width="12.3984375" customWidth="1"/>
+    <col min="33" max="33" width="23.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:38" s="29" customFormat="1" ht="28.9" customHeight="1" thickBot="1">
+      <c r="A1" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="S1" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="T1" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="U1" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="V1" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="W1" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="X1" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA1" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB1" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC1" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD1" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE1" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="AF1" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG1" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH1" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="AI1" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="AJ1" s="28" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38">
+      <c r="A2" s="24" t="s">
         <v>144</v>
       </c>
       <c r="B2" s="24" t="s">
@@ -6178,7 +7032,7 @@
         <v>0.3</v>
       </c>
       <c r="AD2" s="23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE2" s="23" t="b">
         <v>0</v>
@@ -6292,7 +7146,7 @@
         <v>0.3</v>
       </c>
       <c r="AD3" s="23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE3" s="23" t="b">
         <v>1</v>
@@ -6406,7 +7260,7 @@
         <v>0.3</v>
       </c>
       <c r="AD4" s="23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="23" t="b">
         <v>1</v>
@@ -6520,7 +7374,7 @@
         <v>0.3</v>
       </c>
       <c r="AD5" s="23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE5" s="23" t="b">
         <v>1</v>
@@ -6634,7 +7488,7 @@
         <v>0.3</v>
       </c>
       <c r="AD6" s="23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE6" s="23" t="b">
         <v>1</v>
@@ -6748,7 +7602,7 @@
         <v>0.3</v>
       </c>
       <c r="AD7" s="23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE7" s="23" t="b">
         <v>1</v>
@@ -6862,7 +7716,7 @@
         <v>0.3</v>
       </c>
       <c r="AD8" s="23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE8" s="23" t="b">
         <v>1</v>
@@ -6889,10 +7743,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AD2:AG8">
-    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -6904,7 +7758,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ5:AJ8">
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="8">
@@ -6919,7 +7773,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ3">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">
@@ -6934,7 +7788,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ2">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="4">
@@ -6949,7 +7803,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ4">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">
@@ -6967,7 +7821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -7138,7 +7992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -7310,7 +8164,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
@@ -7961,21 +8815,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
-    <tabColor theme="4"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S37" sqref="S37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updates to input file
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_Master_LC_GEP_original.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_Master_LC_GEP_original.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4665FAFF-B628-41A0-830A-96BBE2BE67FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1D3E7C-CEC4-492F-B856-75DA2377D813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="927" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="927" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LC_GEP Setting" sheetId="1" r:id="rId1"/>
@@ -5731,8 +5731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AM6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6225,7 +6225,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="19">
-        <v>5.6829999999999998</v>
+        <v>5683</v>
       </c>
       <c r="N5" s="19">
         <v>4.5</v>
@@ -6673,7 +6673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
extending PTC specification to include a column for nuclear
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_Master_LC_GEP_original.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_Master_LC_GEP_original.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1D3E7C-CEC4-492F-B856-75DA2377D813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D494AD9-2953-436C-9C91-F6BEBE275EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="927" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="927" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LC_GEP Setting" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="288">
   <si>
     <t>Setting</t>
   </si>
@@ -927,6 +927,12 @@
   </si>
   <si>
     <t>AdvancedNuclear</t>
+  </si>
+  <si>
+    <t>PTC_Nuc</t>
+  </si>
+  <si>
+    <t>ITC_Nuc</t>
   </si>
 </sst>
 </file>
@@ -5549,10 +5555,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5564,7 +5570,7 @@
     <col min="27" max="27" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="24" customFormat="1" ht="28.9" customHeight="1" thickBot="1">
+    <row r="1" spans="1:26" s="24" customFormat="1" ht="28.9" customHeight="1" thickBot="1">
       <c r="A1" s="32" t="s">
         <v>58</v>
       </c>
@@ -5637,9 +5643,14 @@
       <c r="X1" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="Y1" s="32"/>
-    </row>
-    <row r="2" spans="1:25">
+      <c r="Y1" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="Z1" s="24" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" s="1" t="s">
         <v>284</v>
       </c>
@@ -5712,7 +5723,12 @@
       <c r="X2" s="1">
         <v>0</v>
       </c>
-      <c r="Y2" s="1"/>
+      <c r="Y2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
@@ -5731,7 +5747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AM6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>

</xml_diff>